<commit_message>
Add new functions for looping
</commit_message>
<xml_diff>
--- a/for-sale/forsale1.xlsx
+++ b/for-sale/forsale1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bpa/Desktop/projects/personal/consumer-debt-portfolio-cleaner/for-sale/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5151B2D1-5A78-A54F-8CFB-C9261A61B24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6AAA04-5C8C-AE4F-BF8B-02AEBC22F72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15940" xr2:uid="{2B336F2D-9304-D04D-808B-46023A8BD6BD}"/>
   </bookViews>
@@ -386,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77CF931-1A29-CE4D-93AD-D97A25B968A9}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="186" workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -474,6 +474,11 @@
         <v>234567</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>